<commit_message>
Excel com alguns grafos
</commit_message>
<xml_diff>
--- a/Grafos e Matrizes de Adjacencia.xlsx
+++ b/Grafos e Matrizes de Adjacencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GW\Documents\GitHub\puc-materia-fmc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83031AD-D4EE-4C6C-A478-43AFE1CD8CF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C28404-ADB5-4C72-A127-BAA2ACC06386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3285" windowWidth="28800" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Grafo C#:</t>
+  </si>
+  <si>
+    <t>Caminho Euleriano:</t>
+  </si>
+  <si>
+    <t>Circuito/Caminho:</t>
+  </si>
+  <si>
+    <t>Nao Euleriano:</t>
+  </si>
+  <si>
+    <t>Grafo Databases:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,6 +63,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -90,19 +110,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -135,7 +163,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>504458</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>114165</xdr:rowOff>
+      <xdr:rowOff>76065</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -160,6 +188,50 @@
         <a:xfrm>
           <a:off x="3057525" y="190500"/>
           <a:ext cx="2933333" cy="1076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>109963</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{119B8E81-86BE-4847-8572-5451F09D0880}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13573126" y="5410201"/>
+          <a:ext cx="4486274" cy="4701012"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -434,35 +506,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M6"/>
+  <dimension ref="A2:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:U48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="1"/>
+    <col min="1" max="1" width="20.5703125" style="5" customWidth="1"/>
+    <col min="2" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="9.140625" style="1" customWidth="1"/>
     <col min="8" max="9" width="9.140625" style="1"/>
+    <col min="11" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="9.28515625" style="1" customWidth="1"/>
+    <col min="18" max="21" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" s="1">
@@ -476,11 +552,11 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -490,11 +566,11 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -503,8 +579,1637 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M6" s="2"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M6" s="6"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="7">
+        <v>1</v>
+      </c>
+      <c r="C28" s="7">
+        <v>2</v>
+      </c>
+      <c r="D28" s="7">
+        <v>3</v>
+      </c>
+      <c r="E28" s="7">
+        <v>4</v>
+      </c>
+      <c r="F28" s="7">
+        <v>5</v>
+      </c>
+      <c r="G28" s="7">
+        <v>6</v>
+      </c>
+      <c r="H28" s="7">
+        <v>7</v>
+      </c>
+      <c r="I28" s="7">
+        <v>8</v>
+      </c>
+      <c r="J28" s="7">
+        <v>9</v>
+      </c>
+      <c r="K28" s="7">
+        <v>10</v>
+      </c>
+      <c r="L28" s="7">
+        <v>11</v>
+      </c>
+      <c r="M28" s="7">
+        <v>12</v>
+      </c>
+      <c r="N28" s="7">
+        <v>13</v>
+      </c>
+      <c r="O28" s="7">
+        <v>14</v>
+      </c>
+      <c r="P28" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>16</v>
+      </c>
+      <c r="R28" s="7">
+        <v>17</v>
+      </c>
+      <c r="S28" s="7">
+        <v>18</v>
+      </c>
+      <c r="T28" s="7">
+        <v>19</v>
+      </c>
+      <c r="U28" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1">
+        <v>0</v>
+      </c>
+      <c r="P29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0</v>
+      </c>
+      <c r="R29" s="1">
+        <v>0</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0</v>
+      </c>
+      <c r="T29" s="1">
+        <v>0</v>
+      </c>
+      <c r="U29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1">
+        <v>0</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0</v>
+      </c>
+      <c r="O30" s="1">
+        <v>0</v>
+      </c>
+      <c r="P30" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>0</v>
+      </c>
+      <c r="R30" s="1">
+        <v>0</v>
+      </c>
+      <c r="S30" s="1">
+        <v>0</v>
+      </c>
+      <c r="T30" s="1">
+        <v>0</v>
+      </c>
+      <c r="U30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>3</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1</v>
+      </c>
+      <c r="L31" s="1">
+        <v>1</v>
+      </c>
+      <c r="M31" s="1">
+        <v>0</v>
+      </c>
+      <c r="N31" s="1">
+        <v>0</v>
+      </c>
+      <c r="O31" s="1">
+        <v>0</v>
+      </c>
+      <c r="P31" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>0</v>
+      </c>
+      <c r="R31" s="1">
+        <v>0</v>
+      </c>
+      <c r="S31" s="1">
+        <v>0</v>
+      </c>
+      <c r="T31" s="1">
+        <v>0</v>
+      </c>
+      <c r="U31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0</v>
+      </c>
+      <c r="M32" s="1">
+        <v>1</v>
+      </c>
+      <c r="N32" s="1">
+        <v>1</v>
+      </c>
+      <c r="O32" s="1">
+        <v>1</v>
+      </c>
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>0</v>
+      </c>
+      <c r="R32" s="1">
+        <v>0</v>
+      </c>
+      <c r="S32" s="1">
+        <v>0</v>
+      </c>
+      <c r="T32" s="1">
+        <v>0</v>
+      </c>
+      <c r="U32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0</v>
+      </c>
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>1</v>
+      </c>
+      <c r="R33" s="1">
+        <v>1</v>
+      </c>
+      <c r="S33" s="1">
+        <v>1</v>
+      </c>
+      <c r="T33" s="1">
+        <v>1</v>
+      </c>
+      <c r="U33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>6</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0</v>
+      </c>
+      <c r="O34" s="1">
+        <v>0</v>
+      </c>
+      <c r="P34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>0</v>
+      </c>
+      <c r="R34" s="1">
+        <v>0</v>
+      </c>
+      <c r="S34" s="1">
+        <v>0</v>
+      </c>
+      <c r="T34" s="1">
+        <v>0</v>
+      </c>
+      <c r="U34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>7</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35" s="1">
+        <v>0</v>
+      </c>
+      <c r="M35" s="1">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1">
+        <v>0</v>
+      </c>
+      <c r="O35" s="1">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>0</v>
+      </c>
+      <c r="R35" s="1">
+        <v>0</v>
+      </c>
+      <c r="S35" s="1">
+        <v>0</v>
+      </c>
+      <c r="T35" s="1">
+        <v>0</v>
+      </c>
+      <c r="U35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>8</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>0</v>
+      </c>
+      <c r="R36" s="1">
+        <v>0</v>
+      </c>
+      <c r="S36" s="1">
+        <v>0</v>
+      </c>
+      <c r="T36" s="1">
+        <v>0</v>
+      </c>
+      <c r="U36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0</v>
+      </c>
+      <c r="L37" s="1">
+        <v>0</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1">
+        <v>0</v>
+      </c>
+      <c r="O37" s="1">
+        <v>0</v>
+      </c>
+      <c r="P37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>0</v>
+      </c>
+      <c r="R37" s="1">
+        <v>0</v>
+      </c>
+      <c r="S37" s="1">
+        <v>0</v>
+      </c>
+      <c r="T37" s="1">
+        <v>0</v>
+      </c>
+      <c r="U37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>10</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0</v>
+      </c>
+      <c r="L38" s="1">
+        <v>0</v>
+      </c>
+      <c r="M38" s="1">
+        <v>0</v>
+      </c>
+      <c r="N38" s="1">
+        <v>0</v>
+      </c>
+      <c r="O38" s="1">
+        <v>0</v>
+      </c>
+      <c r="P38" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>0</v>
+      </c>
+      <c r="R38" s="1">
+        <v>0</v>
+      </c>
+      <c r="S38" s="1">
+        <v>0</v>
+      </c>
+      <c r="T38" s="1">
+        <v>0</v>
+      </c>
+      <c r="U38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>11</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0</v>
+      </c>
+      <c r="J39" s="1">
+        <v>0</v>
+      </c>
+      <c r="K39" s="1">
+        <v>0</v>
+      </c>
+      <c r="L39" s="1">
+        <v>0</v>
+      </c>
+      <c r="M39" s="1">
+        <v>0</v>
+      </c>
+      <c r="N39" s="1">
+        <v>0</v>
+      </c>
+      <c r="O39" s="1">
+        <v>0</v>
+      </c>
+      <c r="P39" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>0</v>
+      </c>
+      <c r="R39" s="1">
+        <v>0</v>
+      </c>
+      <c r="S39" s="1">
+        <v>0</v>
+      </c>
+      <c r="T39" s="1">
+        <v>0</v>
+      </c>
+      <c r="U39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0</v>
+      </c>
+      <c r="K40" s="1">
+        <v>0</v>
+      </c>
+      <c r="L40" s="1">
+        <v>0</v>
+      </c>
+      <c r="M40" s="1">
+        <v>0</v>
+      </c>
+      <c r="N40" s="1">
+        <v>0</v>
+      </c>
+      <c r="O40" s="1">
+        <v>0</v>
+      </c>
+      <c r="P40" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>0</v>
+      </c>
+      <c r="R40" s="1">
+        <v>0</v>
+      </c>
+      <c r="S40" s="1">
+        <v>0</v>
+      </c>
+      <c r="T40" s="1">
+        <v>0</v>
+      </c>
+      <c r="U40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>13</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0</v>
+      </c>
+      <c r="K41" s="1">
+        <v>0</v>
+      </c>
+      <c r="L41" s="1">
+        <v>0</v>
+      </c>
+      <c r="M41" s="1">
+        <v>0</v>
+      </c>
+      <c r="N41" s="1">
+        <v>0</v>
+      </c>
+      <c r="O41" s="1">
+        <v>0</v>
+      </c>
+      <c r="P41" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>0</v>
+      </c>
+      <c r="R41" s="1">
+        <v>0</v>
+      </c>
+      <c r="S41" s="1">
+        <v>0</v>
+      </c>
+      <c r="T41" s="1">
+        <v>0</v>
+      </c>
+      <c r="U41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>14</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0</v>
+      </c>
+      <c r="K42" s="1">
+        <v>0</v>
+      </c>
+      <c r="L42" s="1">
+        <v>0</v>
+      </c>
+      <c r="M42" s="1">
+        <v>0</v>
+      </c>
+      <c r="N42" s="1">
+        <v>0</v>
+      </c>
+      <c r="O42" s="1">
+        <v>0</v>
+      </c>
+      <c r="P42" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>0</v>
+      </c>
+      <c r="R42" s="1">
+        <v>0</v>
+      </c>
+      <c r="S42" s="1">
+        <v>0</v>
+      </c>
+      <c r="T42" s="1">
+        <v>0</v>
+      </c>
+      <c r="U42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>15</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0</v>
+      </c>
+      <c r="J43" s="1">
+        <v>0</v>
+      </c>
+      <c r="K43" s="1">
+        <v>0</v>
+      </c>
+      <c r="L43" s="1">
+        <v>0</v>
+      </c>
+      <c r="M43" s="1">
+        <v>0</v>
+      </c>
+      <c r="N43" s="1">
+        <v>0</v>
+      </c>
+      <c r="O43" s="1">
+        <v>0</v>
+      </c>
+      <c r="P43" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>0</v>
+      </c>
+      <c r="R43" s="1">
+        <v>0</v>
+      </c>
+      <c r="S43" s="1">
+        <v>0</v>
+      </c>
+      <c r="T43" s="1">
+        <v>0</v>
+      </c>
+      <c r="U43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>16</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1">
+        <v>0</v>
+      </c>
+      <c r="L44" s="1">
+        <v>0</v>
+      </c>
+      <c r="M44" s="1">
+        <v>0</v>
+      </c>
+      <c r="N44" s="1">
+        <v>0</v>
+      </c>
+      <c r="O44" s="1">
+        <v>0</v>
+      </c>
+      <c r="P44" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>0</v>
+      </c>
+      <c r="R44" s="1">
+        <v>0</v>
+      </c>
+      <c r="S44" s="1">
+        <v>0</v>
+      </c>
+      <c r="T44" s="1">
+        <v>0</v>
+      </c>
+      <c r="U44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>17</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0</v>
+      </c>
+      <c r="L45" s="1">
+        <v>0</v>
+      </c>
+      <c r="M45" s="1">
+        <v>0</v>
+      </c>
+      <c r="N45" s="1">
+        <v>0</v>
+      </c>
+      <c r="O45" s="1">
+        <v>0</v>
+      </c>
+      <c r="P45" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>0</v>
+      </c>
+      <c r="R45" s="1">
+        <v>0</v>
+      </c>
+      <c r="S45" s="1">
+        <v>0</v>
+      </c>
+      <c r="T45" s="1">
+        <v>0</v>
+      </c>
+      <c r="U45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>18</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0</v>
+      </c>
+      <c r="K46" s="1">
+        <v>0</v>
+      </c>
+      <c r="L46" s="1">
+        <v>0</v>
+      </c>
+      <c r="M46" s="1">
+        <v>0</v>
+      </c>
+      <c r="N46" s="1">
+        <v>0</v>
+      </c>
+      <c r="O46" s="1">
+        <v>0</v>
+      </c>
+      <c r="P46" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>0</v>
+      </c>
+      <c r="R46" s="1">
+        <v>0</v>
+      </c>
+      <c r="S46" s="1">
+        <v>0</v>
+      </c>
+      <c r="T46" s="1">
+        <v>0</v>
+      </c>
+      <c r="U46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>19</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0</v>
+      </c>
+      <c r="J47" s="1">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1">
+        <v>0</v>
+      </c>
+      <c r="L47" s="1">
+        <v>0</v>
+      </c>
+      <c r="M47" s="1">
+        <v>0</v>
+      </c>
+      <c r="N47" s="1">
+        <v>0</v>
+      </c>
+      <c r="O47" s="1">
+        <v>0</v>
+      </c>
+      <c r="P47" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>0</v>
+      </c>
+      <c r="R47" s="1">
+        <v>0</v>
+      </c>
+      <c r="S47" s="1">
+        <v>0</v>
+      </c>
+      <c r="T47" s="1">
+        <v>0</v>
+      </c>
+      <c r="U47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>20</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0</v>
+      </c>
+      <c r="K48" s="1">
+        <v>0</v>
+      </c>
+      <c r="L48" s="1">
+        <v>0</v>
+      </c>
+      <c r="M48" s="1">
+        <v>0</v>
+      </c>
+      <c r="N48" s="1">
+        <v>0</v>
+      </c>
+      <c r="O48" s="1">
+        <v>0</v>
+      </c>
+      <c r="P48" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>0</v>
+      </c>
+      <c r="R48" s="1">
+        <v>0</v>
+      </c>
+      <c r="S48" s="1">
+        <v>0</v>
+      </c>
+      <c r="T48" s="1">
+        <v>0</v>
+      </c>
+      <c r="U48" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Arquivo excel com alguns grafos de exemplo
</commit_message>
<xml_diff>
--- a/Grafos e Matrizes de Adjacencia.xlsx
+++ b/Grafos e Matrizes de Adjacencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GW\Documents\GitHub\puc-materia-fmc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C28404-ADB5-4C72-A127-BAA2ACC06386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB3BEDB-C9BF-49B7-9034-B19EF0A56453}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3285" windowWidth="25725" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -508,7 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B29" sqref="B29:U48"/>
     </sheetView>
   </sheetViews>

</xml_diff>